<commit_message>
Added some more figures
</commit_message>
<xml_diff>
--- a/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
+++ b/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="630"/>
+    <workbookView xWindow="6780" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetStats" sheetId="14" r:id="rId1"/>
@@ -16831,7 +16831,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -17050,11 +17049,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124292360"/>
-        <c:axId val="-2140843704"/>
+        <c:axId val="-2114797512"/>
+        <c:axId val="-2124253656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124292360"/>
+        <c:axId val="-2114797512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17084,7 +17083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2140843704"/>
+        <c:crossAx val="-2124253656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17092,7 +17091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2140843704"/>
+        <c:axId val="-2124253656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17113,7 +17112,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124292360"/>
+        <c:crossAx val="-2114797512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17160,7 +17159,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -17372,11 +17370,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124079240"/>
-        <c:axId val="-2124387800"/>
+        <c:axId val="-2124343528"/>
+        <c:axId val="-2122355848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124079240"/>
+        <c:axId val="-2124343528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17406,7 +17404,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124387800"/>
+        <c:crossAx val="-2122355848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17414,7 +17412,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124387800"/>
+        <c:axId val="-2122355848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2600.0"/>
@@ -17437,7 +17435,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124079240"/>
+        <c:crossAx val="-2124343528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17475,8 +17473,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0636516695255613"/>
-          <c:y val="0.070631970260223"/>
+          <c:x val="0.0636516685414323"/>
+          <c:y val="0.0886500673902248"/>
           <c:w val="0.636069034306156"/>
           <c:h val="0.45104557562275"/>
         </c:manualLayout>
@@ -18488,11 +18486,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123703496"/>
-        <c:axId val="-2124221832"/>
+        <c:axId val="-2124214600"/>
+        <c:axId val="-2140978216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123703496"/>
+        <c:axId val="-2124214600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18524,7 +18522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124221832"/>
+        <c:crossAx val="-2140978216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18532,7 +18530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124221832"/>
+        <c:axId val="-2140978216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -18577,7 +18575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123703496"/>
+        <c:crossAx val="-2124214600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -18589,9 +18587,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.000505811773528309"/>
-          <c:y val="0.0"/>
-          <c:w val="0.746657042869641"/>
+          <c:x val="0.0238095238095238"/>
+          <c:y val="0.024024024024024"/>
+          <c:w val="0.683164979377578"/>
           <c:h val="0.060309049206687"/>
         </c:manualLayout>
       </c:layout>
@@ -19045,7 +19043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+    <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D26"/>
     </sheetView>
   </sheetViews>
@@ -20031,7 +20029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added the figure on feature improvements and some more references
</commit_message>
<xml_diff>
--- a/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
+++ b/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5169" uniqueCount="4967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5170" uniqueCount="4967">
   <si>
     <t>appliances</t>
   </si>
@@ -15010,7 +15010,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="880">
+  <cellStyleXfs count="886">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -15891,6 +15891,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -15910,7 +15916,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="880">
+  <cellStyles count="886">
     <cellStyle name="Comma 2" xfId="95"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -16351,6 +16357,9 @@
     <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="877" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="879" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="881" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="883" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="885" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -16790,6 +16799,9 @@
     <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="876" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="878" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="880" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="882" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="884" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -17060,11 +17072,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2002537608"/>
-        <c:axId val="-2002513768"/>
+        <c:axId val="-2145633944"/>
+        <c:axId val="-1988266248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2002537608"/>
+        <c:axId val="-2145633944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17094,7 +17106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002513768"/>
+        <c:crossAx val="-1988266248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17102,7 +17114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2002513768"/>
+        <c:axId val="-1988266248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17123,7 +17135,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2002537608"/>
+        <c:crossAx val="-2145633944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17382,11 +17394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2002479048"/>
-        <c:axId val="-2002475960"/>
+        <c:axId val="-1988853624"/>
+        <c:axId val="-2131331496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2002479048"/>
+        <c:axId val="-1988853624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17416,7 +17428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002475960"/>
+        <c:crossAx val="-2131331496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17424,7 +17436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2002475960"/>
+        <c:axId val="-2131331496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2600.0"/>
@@ -17447,7 +17459,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2002479048"/>
+        <c:crossAx val="-1988853624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18498,11 +18510,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1988849624"/>
-        <c:axId val="-2002177128"/>
+        <c:axId val="-1988322456"/>
+        <c:axId val="-2002174744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1988849624"/>
+        <c:axId val="-1988322456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18534,7 +18546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002177128"/>
+        <c:crossAx val="-2002174744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18542,7 +18554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2002177128"/>
+        <c:axId val="-2002174744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -18587,7 +18599,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988849624"/>
+        <c:crossAx val="-1988322456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -19056,7 +19068,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19597,6 +19609,10 @@
     <row r="28" spans="1:7">
       <c r="C28" s="1" t="s">
         <v>4965</v>
+      </c>
+      <c r="E28">
+        <f>SUM(E2:E26)</f>
+        <v>18188</v>
       </c>
       <c r="F28">
         <f>SUM(F2:F26)</f>
@@ -20065,7 +20081,7 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:H2"/>
+      <selection activeCell="C2" sqref="C2:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20688,6 +20704,9 @@
       </c>
     </row>
     <row r="28" spans="1:8">
+      <c r="C28" t="s">
+        <v>4966</v>
+      </c>
       <c r="D28" s="3">
         <f>AVERAGE(D3:D27)</f>
         <v>49.013376000000008</v>

</xml_diff>

<commit_message>
Cleaned up the images a bit
</commit_message>
<xml_diff>
--- a/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
+++ b/coling2016/props/AmazonJulian-COLING-2016-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="630"/>
+    <workbookView xWindow="6780" yWindow="660" windowWidth="25600" windowHeight="16060" tabRatio="630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetStats" sheetId="14" r:id="rId1"/>
@@ -17072,11 +17072,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2145633944"/>
-        <c:axId val="-1988266248"/>
+        <c:axId val="-2003069864"/>
+        <c:axId val="-2131657320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145633944"/>
+        <c:axId val="-2003069864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17106,7 +17106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988266248"/>
+        <c:crossAx val="-2131657320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17114,7 +17114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1988266248"/>
+        <c:axId val="-2131657320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17135,7 +17135,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145633944"/>
+        <c:crossAx val="-2003069864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17394,11 +17394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1988853624"/>
-        <c:axId val="-2131331496"/>
+        <c:axId val="-2002428312"/>
+        <c:axId val="-2003792088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1988853624"/>
+        <c:axId val="-2002428312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17428,7 +17428,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131331496"/>
+        <c:crossAx val="-2003792088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17436,7 +17436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131331496"/>
+        <c:axId val="-2003792088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2600.0"/>
@@ -17459,7 +17459,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1988853624"/>
+        <c:crossAx val="-2002428312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17497,9 +17497,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0636516685414323"/>
-          <c:y val="0.0886500673902248"/>
-          <c:w val="0.636069034306156"/>
+          <c:x val="0.0842865891763529"/>
+          <c:y val="0.0796410583812159"/>
+          <c:w val="0.698300462442195"/>
           <c:h val="0.45104557562275"/>
         </c:manualLayout>
       </c:layout>
@@ -18510,11 +18510,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1988322456"/>
-        <c:axId val="-2002174744"/>
+        <c:axId val="-2003712328"/>
+        <c:axId val="-2130800280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1988322456"/>
+        <c:axId val="-2003712328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18526,9 +18526,8 @@
         <c:spPr>
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
                 <a:alpha val="43000"/>
               </a:schemeClr>
             </a:outerShdw>
@@ -18541,12 +18540,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" baseline="0"/>
+              <a:defRPr sz="1400" baseline="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002174744"/>
+        <c:crossAx val="-2130800280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18554,7 +18553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2002174744"/>
+        <c:axId val="-2130800280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -18579,27 +18578,19 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="43000"/>
-              </a:schemeClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" baseline="0"/>
+              <a:defRPr sz="1400" baseline="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988322456"/>
+        <c:crossAx val="-2003712328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -18611,10 +18602,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0238095238095238"/>
-          <c:y val="0.024024024024024"/>
-          <c:w val="0.683164979377578"/>
-          <c:h val="0.060309049206687"/>
+          <c:x val="0.0492063492063492"/>
+          <c:y val="0.021021021021021"/>
+          <c:w val="0.73554593175853"/>
+          <c:h val="0.06331205220969"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -18623,7 +18614,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" kern="1200" baseline="0"/>
+            <a:defRPr sz="1200" kern="1200" baseline="0"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -19067,7 +19058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -20080,8 +20071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>